<commit_message>
:construction: add new table customer and item to PGSQL bdd
</commit_message>
<xml_diff>
--- a/EXCEL/analyseTable.xlsx
+++ b/EXCEL/analyseTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j.serafini\Desktop\Jordan\Code\Back form\EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1047CFC6-94B5-49CE-841D-13BAD75C86FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB56C6D-7097-4241-A066-FD39EB39760B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -420,7 +420,7 @@
   <dimension ref="A1:A31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>